<commit_message>
upd 06.10 - 13.10
Методы оптимизации - лаба 2
Системный анализ - лаба 2 upd, 3
Философия - +2 анализа текста
Архитектура - лекция 3
</commit_message>
<xml_diff>
--- a/Системный анализ/Лаб 1/lab1_Модули AgileCRM(Системный анализ).xlsx
+++ b/Системный анализ/Лаб 1/lab1_Модули AgileCRM(Системный анализ).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Shelty\ITMO-Lecture-5-sem\Системный анализ\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Shelty\ITMO-5-sem\Системный анализ\Лаб 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47CD0E3B-50D0-4540-AE13-FDF08303ED78}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F72FF35-816E-4A50-8145-45B069F5A81A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{9E721E86-1C62-4940-A84E-AD96A574D3AC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{9E721E86-1C62-4940-A84E-AD96A574D3AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Элементы" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="103">
   <si>
     <t>Название элемента</t>
   </si>
@@ -335,13 +335,19 @@
   </si>
   <si>
     <t>Данные о сделках</t>
+  </si>
+  <si>
+    <t>Отправка сообщения клиенту</t>
+  </si>
+  <si>
+    <t>Клиентская информация</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -353,22 +359,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="9"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="9" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -470,7 +460,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -492,13 +482,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -815,8 +801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C969B7D0-FDFE-4449-BCF4-2DBAFF3E8B17}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="A17:B17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1213,10 +1199,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C7F51E-532C-4CA3-9CB6-BE17CCE0DCCA}">
-  <dimension ref="A1:L51"/>
+  <dimension ref="A1:L53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1570,36 +1556,36 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="10">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B21" s="10">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C21" s="9">
         <v>20</v>
       </c>
-      <c r="D21" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>67</v>
+      <c r="D21" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" s="9">
-        <v>10</v>
-      </c>
-      <c r="B22" s="10">
-        <v>5</v>
+      <c r="A22" s="17">
+        <v>20</v>
+      </c>
+      <c r="B22" s="16">
+        <v>17</v>
       </c>
       <c r="C22" s="9">
         <v>21</v>
       </c>
-      <c r="D22" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>35</v>
+      <c r="D22" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
@@ -1637,24 +1623,24 @@
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A25" s="9">
+      <c r="A25" s="15">
         <v>12</v>
       </c>
-      <c r="B25" s="10">
+      <c r="B25" s="16">
         <v>8</v>
       </c>
-      <c r="C25" s="9">
+      <c r="C25" s="15">
         <v>24</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D25" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="E25" s="15" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A26" s="15">
+      <c r="A26" s="17">
         <v>16</v>
       </c>
       <c r="B26" s="16">
@@ -1663,91 +1649,71 @@
       <c r="C26" s="16">
         <v>25</v>
       </c>
-      <c r="D26" s="17" t="s">
+      <c r="D26" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="E26" s="17" t="s">
+      <c r="E26" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="H26" s="13">
-        <v>12</v>
-      </c>
-      <c r="I26" s="14">
-        <v>19</v>
-      </c>
-      <c r="J26" s="13">
-        <v>25</v>
-      </c>
-      <c r="K26" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="L26" s="13" t="s">
-        <v>35</v>
-      </c>
+      <c r="H26" s="13"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="13"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A27" s="15">
-        <v>20</v>
+      <c r="A27" s="8">
+        <v>16</v>
       </c>
       <c r="B27" s="16">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C27" s="16">
         <v>26</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="E27" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="H27" s="13">
-        <v>19</v>
-      </c>
-      <c r="I27" s="14">
-        <v>12</v>
-      </c>
-      <c r="J27" s="13">
-        <v>26</v>
-      </c>
-      <c r="K27" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="L27" s="14" t="s">
-        <v>67</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="H27" s="13"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="14"/>
+      <c r="L27" s="14"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A28" s="9">
+      <c r="A28" s="15">
         <v>9</v>
       </c>
-      <c r="B28" s="10">
+      <c r="B28" s="16">
         <v>11</v>
       </c>
-      <c r="C28" s="9">
+      <c r="C28" s="15">
         <v>27</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="D28" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="E28" s="9" t="s">
+      <c r="E28" s="15" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A29" s="9">
+      <c r="A29" s="15">
         <v>11</v>
       </c>
-      <c r="B29" s="10">
+      <c r="B29" s="16">
         <v>9</v>
       </c>
-      <c r="C29" s="9">
+      <c r="C29" s="15">
         <v>28</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D29" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="E29" s="9" t="s">
+      <c r="E29" s="15" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1769,19 +1735,19 @@
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A31" s="20">
+      <c r="A31" s="15">
         <v>10</v>
       </c>
-      <c r="B31" s="21">
+      <c r="B31" s="16">
         <v>11</v>
       </c>
-      <c r="C31" s="20">
+      <c r="C31" s="15">
         <v>30</v>
       </c>
       <c r="D31" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="E31" s="20" t="s">
+      <c r="E31" s="15" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1888,19 +1854,19 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="20">
+      <c r="A38" s="15">
         <v>17</v>
       </c>
-      <c r="B38" s="21">
+      <c r="B38" s="16">
         <v>16</v>
       </c>
-      <c r="C38" s="20">
+      <c r="C38" s="15">
         <v>37</v>
       </c>
-      <c r="D38" s="21" t="s">
+      <c r="D38" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E38" s="21" t="s">
+      <c r="E38" s="16" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1922,20 +1888,20 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="9">
-        <v>17</v>
-      </c>
-      <c r="B40" s="10">
-        <v>19</v>
+      <c r="A40" s="17">
+        <v>16</v>
+      </c>
+      <c r="B40" s="16">
+        <v>20</v>
       </c>
       <c r="C40" s="9">
         <v>39</v>
       </c>
-      <c r="D40" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>35</v>
+      <c r="D40" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="E40" s="16" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -2007,123 +1973,119 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="9">
-        <v>19</v>
-      </c>
-      <c r="B45" s="10">
-        <v>17</v>
+      <c r="A45" s="17">
+        <v>12</v>
+      </c>
+      <c r="B45" s="16">
+        <v>16</v>
       </c>
       <c r="C45" s="10">
         <v>44</v>
       </c>
-      <c r="D45" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="E45" s="10" t="s">
-        <v>67</v>
+      <c r="D45" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="E45" s="16" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="9">
+      <c r="A46" s="15">
         <v>17</v>
       </c>
-      <c r="B46" s="10">
+      <c r="B46" s="16">
         <v>21</v>
       </c>
-      <c r="C46" s="10">
+      <c r="C46" s="16">
         <v>45</v>
       </c>
-      <c r="D46" s="10" t="s">
+      <c r="D46" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="E46" s="9" t="s">
+      <c r="E46" s="15" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="9">
+      <c r="A47" s="15">
         <v>21</v>
       </c>
-      <c r="B47" s="10">
+      <c r="B47" s="16">
         <v>17</v>
       </c>
-      <c r="C47" s="10">
+      <c r="C47" s="16">
         <v>46</v>
       </c>
-      <c r="D47" s="10" t="s">
+      <c r="D47" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="E47" s="10" t="s">
+      <c r="E47" s="16" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="18">
+      <c r="A48" s="17">
         <v>10</v>
       </c>
-      <c r="B48" s="19">
+      <c r="B48" s="16">
         <v>12</v>
       </c>
-      <c r="C48" s="19">
+      <c r="C48" s="16">
         <v>47</v>
       </c>
-      <c r="D48" s="19" t="s">
+      <c r="D48" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="E48" s="19" t="s">
+      <c r="E48" s="16" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="18">
+      <c r="A49" s="17">
         <v>10</v>
       </c>
-      <c r="B49" s="19">
+      <c r="B49" s="16">
         <v>9</v>
       </c>
-      <c r="C49" s="19">
+      <c r="C49" s="16">
         <v>48</v>
       </c>
-      <c r="D49" s="19" t="s">
+      <c r="D49" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="E49" s="19" t="s">
+      <c r="E49" s="16" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="18">
+      <c r="A50" s="17">
         <v>10</v>
       </c>
-      <c r="B50" s="19">
+      <c r="B50" s="16">
         <v>13</v>
       </c>
-      <c r="C50" s="19">
+      <c r="C50" s="16">
         <v>49</v>
       </c>
-      <c r="D50" s="19" t="s">
+      <c r="D50" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="E50" s="19" t="s">
+      <c r="E50" s="16" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" s="18">
-        <v>12</v>
-      </c>
-      <c r="B51" s="19">
-        <v>16</v>
-      </c>
-      <c r="C51" s="19">
-        <v>50</v>
-      </c>
-      <c r="D51" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="E51" s="19" t="s">
-        <v>83</v>
-      </c>
+      <c r="C51" s="16"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C52" s="16"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="17"/>
+      <c r="B53" s="15"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2136,7 +2098,7 @@
   <dimension ref="A1:V22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection sqref="A1:V22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2343,9 +2305,7 @@
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
-      <c r="K6" s="9">
-        <v>1</v>
-      </c>
+      <c r="K6" s="9"/>
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
       <c r="N6" s="9">
@@ -2483,9 +2443,7 @@
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
-      <c r="F11" s="9">
-        <v>1</v>
-      </c>
+      <c r="F11" s="9"/>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
@@ -2666,7 +2624,9 @@
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
+      <c r="K17" s="9">
+        <v>1</v>
+      </c>
       <c r="L17" s="9"/>
       <c r="M17" s="9"/>
       <c r="N17" s="9"/>
@@ -2680,7 +2640,9 @@
       </c>
       <c r="S17" s="9"/>
       <c r="T17" s="9"/>
-      <c r="U17" s="9"/>
+      <c r="U17" s="9">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18" s="9">
@@ -2710,10 +2672,10 @@
       </c>
       <c r="R18" s="9"/>
       <c r="S18" s="9"/>
-      <c r="T18" s="9">
-        <v>1</v>
-      </c>
-      <c r="U18" s="9"/>
+      <c r="T18" s="9"/>
+      <c r="U18" s="9">
+        <v>1</v>
+      </c>
       <c r="V18">
         <v>1</v>
       </c>
@@ -2769,9 +2731,7 @@
       <c r="O20" s="9"/>
       <c r="P20" s="9"/>
       <c r="Q20" s="9"/>
-      <c r="R20" s="9">
-        <v>1</v>
-      </c>
+      <c r="R20" s="9"/>
       <c r="S20" s="9"/>
       <c r="T20" s="9"/>
       <c r="U20" s="9">

</xml_diff>